<commit_message>
This was the original dataset before the modifications of bedrooms number where property type was vacant land
</commit_message>
<xml_diff>
--- a/Nairobi property.xlsx
+++ b/Nairobi property.xlsx
@@ -627,19 +627,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -675,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -686,9 +680,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -696,7 +687,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,16 +997,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1048,10 +1039,10 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
         <v>4</v>
       </c>
       <c r="F2" s="2"/>
@@ -1069,9 +1060,7 @@
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4">
-        <f>IF(B3= "Vacant Land", 0, D3)</f>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="1" t="s">
@@ -1088,9 +1077,7 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4">
-        <f>IF(B4= "Vacant Land", 0, D4)</f>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
@@ -1107,10 +1094,10 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>5</v>
       </c>
       <c r="F5" s="2"/>
@@ -1128,10 +1115,10 @@
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4">
-        <v>4</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1149,10 +1136,10 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>6</v>
       </c>
       <c r="F7" s="2"/>
@@ -1170,10 +1157,10 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
         <v>4</v>
       </c>
       <c r="F8" s="2"/>
@@ -1191,10 +1178,10 @@
       <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1212,10 +1199,10 @@
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
         <v>4</v>
       </c>
       <c r="F10" s="2"/>
@@ -1223,7 +1210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1233,10 +1220,10 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1244,7 +1231,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1254,10 +1241,10 @@
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>5</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>4</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -1265,7 +1252,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1275,10 +1262,10 @@
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>5</v>
       </c>
       <c r="F13" s="2"/>
@@ -1296,10 +1283,10 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="4">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
         <v>4</v>
       </c>
       <c r="F14" s="2"/>
@@ -1317,10 +1304,10 @@
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="2">
         <v>6</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>6</v>
       </c>
       <c r="F15" s="2"/>
@@ -1338,10 +1325,10 @@
       <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="2">
         <v>6</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>6</v>
       </c>
       <c r="F16" s="2"/>
@@ -1359,10 +1346,10 @@
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="4">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4">
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1380,10 +1367,10 @@
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="4">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4">
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
         <v>2</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -1401,10 +1388,10 @@
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="4">
-        <v>2</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -1422,10 +1409,10 @@
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="4">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
         <v>8</v>
       </c>
       <c r="F20" s="2"/>
@@ -1443,10 +1430,10 @@
       <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="4">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4">
+      <c r="D21" s="2">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2">
         <v>3</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -1464,10 +1451,10 @@
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="4">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4">
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
         <v>2</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -1485,10 +1472,10 @@
       <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="4">
-        <v>4</v>
-      </c>
-      <c r="E23" s="4">
+      <c r="D23" s="2">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
         <v>3</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -1506,10 +1493,10 @@
       <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="4">
-        <v>3</v>
-      </c>
-      <c r="E24" s="4">
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
         <v>4</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -1527,10 +1514,10 @@
       <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="2">
         <v>5</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="2">
         <v>4</v>
       </c>
       <c r="F25" s="2"/>
@@ -1548,9 +1535,7 @@
       <c r="C26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="4">
-        <f>IF(B3= "Vacant Land", 0, D3)</f>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="1" t="s">
@@ -1567,10 +1552,10 @@
       <c r="C27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="2">
         <v>6</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="2">
         <v>6</v>
       </c>
       <c r="F27" s="2"/>
@@ -1588,10 +1573,10 @@
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="4">
-        <v>8</v>
-      </c>
-      <c r="E28" s="4">
+      <c r="D28" s="2">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2">
         <v>7</v>
       </c>
       <c r="F28" s="2"/>
@@ -1609,10 +1594,10 @@
       <c r="C29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="4">
-        <v>4</v>
-      </c>
-      <c r="E29" s="4">
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
         <v>4</v>
       </c>
       <c r="F29" s="2"/>
@@ -1630,10 +1615,10 @@
       <c r="C30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="2">
         <v>5</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="2">
         <v>3</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -1651,10 +1636,10 @@
       <c r="C31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="2">
         <v>5</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <v>4</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -1672,10 +1657,10 @@
       <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="4">
-        <v>3</v>
-      </c>
-      <c r="E32" s="4">
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2">
         <v>2</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -1693,10 +1678,10 @@
       <c r="C33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>5</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <v>3</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1714,10 +1699,10 @@
       <c r="C34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="4">
-        <v>2</v>
-      </c>
-      <c r="E34" s="4">
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
         <v>2</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -1769,10 +1754,10 @@
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="4">
-        <v>2</v>
-      </c>
-      <c r="E37" s="4">
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2">
         <v>2</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1790,10 +1775,10 @@
       <c r="C38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="4">
-        <v>4</v>
-      </c>
-      <c r="E38" s="4">
+      <c r="D38" s="2">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2">
         <v>3</v>
       </c>
       <c r="F38" s="2"/>
@@ -1828,10 +1813,10 @@
       <c r="C40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="2">
         <v>1</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="2">
         <v>1</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -1849,10 +1834,10 @@
       <c r="C41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="4">
-        <v>4</v>
-      </c>
-      <c r="E41" s="4">
+      <c r="D41" s="2">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2">
         <v>3</v>
       </c>
       <c r="F41" s="2"/>
@@ -1870,10 +1855,10 @@
       <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="4">
-        <v>4</v>
-      </c>
-      <c r="E42" s="4">
+      <c r="D42" s="2">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2">
         <v>4</v>
       </c>
       <c r="F42" s="2"/>
@@ -1908,10 +1893,10 @@
       <c r="C44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="4">
-        <v>2</v>
-      </c>
-      <c r="E44" s="4">
+      <c r="D44" s="2">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2">
         <v>2</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -1929,10 +1914,10 @@
       <c r="C45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="2">
         <v>1</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="2">
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -1950,10 +1935,10 @@
       <c r="C46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="4">
-        <v>2</v>
-      </c>
-      <c r="E46" s="4">
+      <c r="D46" s="2">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2">
         <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1971,10 +1956,10 @@
       <c r="C47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="4">
-        <v>2</v>
-      </c>
-      <c r="E47" s="4">
+      <c r="D47" s="2">
+        <v>2</v>
+      </c>
+      <c r="E47" s="2">
         <v>1</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -1992,10 +1977,10 @@
       <c r="C48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="4">
-        <v>8</v>
-      </c>
-      <c r="E48" s="4">
+      <c r="D48" s="2">
+        <v>8</v>
+      </c>
+      <c r="E48" s="2">
         <v>7</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -2013,10 +1998,10 @@
       <c r="C49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="4">
-        <v>4</v>
-      </c>
-      <c r="E49" s="4">
+      <c r="D49" s="2">
+        <v>4</v>
+      </c>
+      <c r="E49" s="2">
         <v>3</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -2034,10 +2019,10 @@
       <c r="C50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="4">
-        <v>2</v>
-      </c>
-      <c r="E50" s="4">
+      <c r="D50" s="2">
+        <v>2</v>
+      </c>
+      <c r="E50" s="2">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -2055,10 +2040,10 @@
       <c r="C51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="4">
-        <v>4</v>
-      </c>
-      <c r="E51" s="4">
+      <c r="D51" s="2">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2">
         <v>4</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -2076,10 +2061,10 @@
       <c r="C52" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="2">
         <v>5</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="2">
         <v>4</v>
       </c>
       <c r="F52" s="2"/>
@@ -2097,10 +2082,10 @@
       <c r="C53" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="2">
         <v>5</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="2">
         <v>3</v>
       </c>
       <c r="F53" s="2"/>
@@ -2118,10 +2103,10 @@
       <c r="C54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="4">
-        <v>3</v>
-      </c>
-      <c r="E54" s="4">
+      <c r="D54" s="2">
+        <v>3</v>
+      </c>
+      <c r="E54" s="2">
         <v>2</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -2139,10 +2124,10 @@
       <c r="C55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="4">
-        <v>4</v>
-      </c>
-      <c r="E55" s="4">
+      <c r="D55" s="2">
+        <v>4</v>
+      </c>
+      <c r="E55" s="2">
         <v>4</v>
       </c>
       <c r="F55" s="2"/>
@@ -2160,10 +2145,10 @@
       <c r="C56" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="4">
-        <v>2</v>
-      </c>
-      <c r="E56" s="4">
+      <c r="D56" s="2">
+        <v>2</v>
+      </c>
+      <c r="E56" s="2">
         <v>2</v>
       </c>
       <c r="F56" s="3" t="s">
@@ -2181,10 +2166,10 @@
       <c r="C57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="4">
-        <v>4</v>
-      </c>
-      <c r="E57" s="4">
+      <c r="D57" s="2">
+        <v>4</v>
+      </c>
+      <c r="E57" s="2">
         <v>4</v>
       </c>
       <c r="F57" s="2"/>
@@ -2202,10 +2187,10 @@
       <c r="C58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D58" s="4">
-        <v>2</v>
-      </c>
-      <c r="E58" s="4">
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+      <c r="E58" s="2">
         <v>1</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -2223,10 +2208,10 @@
       <c r="C59" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="4">
-        <v>2</v>
-      </c>
-      <c r="E59" s="4">
+      <c r="D59" s="2">
+        <v>2</v>
+      </c>
+      <c r="E59" s="2">
         <v>1</v>
       </c>
       <c r="F59" s="3" t="s">
@@ -2244,10 +2229,10 @@
       <c r="C60" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D60" s="4">
-        <v>2</v>
-      </c>
-      <c r="E60" s="4">
+      <c r="D60" s="2">
+        <v>2</v>
+      </c>
+      <c r="E60" s="2">
         <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
@@ -2265,10 +2250,10 @@
       <c r="C61" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D61" s="4">
-        <v>3</v>
-      </c>
-      <c r="E61" s="4">
+      <c r="D61" s="2">
+        <v>3</v>
+      </c>
+      <c r="E61" s="2">
         <v>2</v>
       </c>
       <c r="F61" s="3" t="s">
@@ -2286,10 +2271,10 @@
       <c r="C62" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="4">
-        <v>2</v>
-      </c>
-      <c r="E62" s="4">
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
+      <c r="E62" s="2">
         <v>2</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -2307,10 +2292,10 @@
       <c r="C63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D63" s="2">
         <v>5</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="2">
         <v>2</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -2328,10 +2313,10 @@
       <c r="C64" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="4">
-        <v>3</v>
-      </c>
-      <c r="E64" s="4">
+      <c r="D64" s="2">
+        <v>3</v>
+      </c>
+      <c r="E64" s="2">
         <v>2</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -2349,10 +2334,10 @@
       <c r="C65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="4">
-        <v>2</v>
-      </c>
-      <c r="E65" s="4">
+      <c r="D65" s="2">
+        <v>2</v>
+      </c>
+      <c r="E65" s="2">
         <v>1</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -2370,10 +2355,10 @@
       <c r="C66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="4">
-        <v>3</v>
-      </c>
-      <c r="E66" s="4">
+      <c r="D66" s="2">
+        <v>3</v>
+      </c>
+      <c r="E66" s="2">
         <v>2</v>
       </c>
       <c r="F66" s="3" t="s">
@@ -2391,10 +2376,10 @@
       <c r="C67" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D67" s="4">
-        <v>2</v>
-      </c>
-      <c r="E67" s="4">
+      <c r="D67" s="2">
+        <v>2</v>
+      </c>
+      <c r="E67" s="2">
         <v>1</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -2429,10 +2414,10 @@
       <c r="C69" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D69" s="4">
-        <v>4</v>
-      </c>
-      <c r="E69" s="4">
+      <c r="D69" s="2">
+        <v>4</v>
+      </c>
+      <c r="E69" s="2">
         <v>2</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -2450,10 +2435,10 @@
       <c r="C70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="4">
-        <v>4</v>
-      </c>
-      <c r="E70" s="4">
+      <c r="D70" s="2">
+        <v>4</v>
+      </c>
+      <c r="E70" s="2">
         <v>2</v>
       </c>
       <c r="F70" s="3" t="s">
@@ -2471,10 +2456,10 @@
       <c r="C71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D71" s="2">
         <v>5</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="2">
         <v>3</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -2492,10 +2477,10 @@
       <c r="C72" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="4">
-        <v>4</v>
-      </c>
-      <c r="E72" s="4">
+      <c r="D72" s="2">
+        <v>4</v>
+      </c>
+      <c r="E72" s="2">
         <v>2</v>
       </c>
       <c r="F72" s="3" t="s">
@@ -2513,10 +2498,10 @@
       <c r="C73" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="2">
         <v>1</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="2">
         <v>1</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -2534,10 +2519,10 @@
       <c r="C74" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D74" s="2">
         <v>1</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="2">
         <v>1</v>
       </c>
       <c r="F74" s="3" t="s">
@@ -2555,10 +2540,10 @@
       <c r="C75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="4">
-        <v>2</v>
-      </c>
-      <c r="E75" s="4">
+      <c r="D75" s="2">
+        <v>2</v>
+      </c>
+      <c r="E75" s="2">
         <v>2</v>
       </c>
       <c r="F75" s="3" t="s">
@@ -2593,10 +2578,10 @@
       <c r="C77" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="4">
-        <v>3</v>
-      </c>
-      <c r="E77" s="4">
+      <c r="D77" s="2">
+        <v>3</v>
+      </c>
+      <c r="E77" s="2">
         <v>2</v>
       </c>
       <c r="F77" s="3" t="s">
@@ -2665,10 +2650,10 @@
       <c r="C81" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D81" s="4">
-        <v>4</v>
-      </c>
-      <c r="E81" s="4">
+      <c r="D81" s="2">
+        <v>4</v>
+      </c>
+      <c r="E81" s="2">
         <v>4</v>
       </c>
       <c r="F81" s="3" t="s">
@@ -2688,10 +2673,10 @@
       <c r="C82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D82" s="4">
-        <v>8</v>
-      </c>
-      <c r="E82" s="4">
+      <c r="D82" s="2">
+        <v>8</v>
+      </c>
+      <c r="E82" s="2">
         <v>7</v>
       </c>
       <c r="F82" s="3" t="s">
@@ -2709,10 +2694,10 @@
       <c r="C83" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D83" s="4">
-        <v>2</v>
-      </c>
-      <c r="E83" s="4">
+      <c r="D83" s="2">
+        <v>2</v>
+      </c>
+      <c r="E83" s="2">
         <v>2</v>
       </c>
       <c r="F83" s="2"/>
@@ -2730,10 +2715,10 @@
       <c r="C84" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D84" s="2">
         <v>5</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="2">
         <v>5</v>
       </c>
       <c r="F84" s="2"/>
@@ -2785,10 +2770,10 @@
       <c r="C87" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="4">
-        <v>2</v>
-      </c>
-      <c r="E87" s="4">
+      <c r="D87" s="2">
+        <v>2</v>
+      </c>
+      <c r="E87" s="2">
         <v>2</v>
       </c>
       <c r="F87" s="2"/>
@@ -2804,10 +2789,10 @@
       <c r="C88" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D88" s="4">
-        <v>4</v>
-      </c>
-      <c r="E88" s="4">
+      <c r="D88" s="2">
+        <v>4</v>
+      </c>
+      <c r="E88" s="2">
         <v>4</v>
       </c>
       <c r="F88" s="3" t="s">
@@ -2825,10 +2810,10 @@
       <c r="C89" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D89" s="4">
-        <v>4</v>
-      </c>
-      <c r="E89" s="4">
+      <c r="D89" s="2">
+        <v>4</v>
+      </c>
+      <c r="E89" s="2">
         <v>2</v>
       </c>
       <c r="F89" s="3" t="s">
@@ -2846,10 +2831,10 @@
       <c r="C90" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D90" s="4">
-        <v>3</v>
-      </c>
-      <c r="E90" s="4">
+      <c r="D90" s="2">
+        <v>3</v>
+      </c>
+      <c r="E90" s="2">
         <v>2</v>
       </c>
       <c r="F90" s="2"/>
@@ -2884,10 +2869,10 @@
       <c r="C92" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D92" s="2">
         <v>6</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92" s="2">
         <v>6</v>
       </c>
       <c r="F92" s="2"/>
@@ -2905,10 +2890,10 @@
       <c r="C93" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D93" s="2">
         <v>5</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93" s="2">
         <v>5</v>
       </c>
       <c r="F93" s="3" t="s">
@@ -2926,10 +2911,10 @@
       <c r="C94" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D94" s="4">
-        <v>2</v>
-      </c>
-      <c r="E94" s="4">
+      <c r="D94" s="2">
+        <v>2</v>
+      </c>
+      <c r="E94" s="2">
         <v>1</v>
       </c>
       <c r="F94" s="2"/>
@@ -2947,10 +2932,10 @@
       <c r="C95" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D95" s="4">
-        <v>4</v>
-      </c>
-      <c r="E95" s="4">
+      <c r="D95" s="2">
+        <v>4</v>
+      </c>
+      <c r="E95" s="2">
         <v>4</v>
       </c>
       <c r="F95" s="3" t="s">
@@ -2968,13 +2953,13 @@
       <c r="C96" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D96" s="2">
         <v>1</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96" s="2">
         <v>1</v>
       </c>
-      <c r="F96" s="4">
+      <c r="F96" s="2">
         <v>1</v>
       </c>
       <c r="G96" s="1" t="s">
@@ -2991,10 +2976,10 @@
       <c r="C97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D97" s="4">
-        <v>4</v>
-      </c>
-      <c r="E97" s="4">
+      <c r="D97" s="2">
+        <v>4</v>
+      </c>
+      <c r="E97" s="2">
         <v>4</v>
       </c>
       <c r="F97" s="2"/>
@@ -3027,10 +3012,10 @@
       <c r="C99" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D99" s="4">
-        <v>3</v>
-      </c>
-      <c r="E99" s="4">
+      <c r="D99" s="2">
+        <v>3</v>
+      </c>
+      <c r="E99" s="2">
         <v>2</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -3048,10 +3033,10 @@
       <c r="C100" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D100" s="4">
-        <v>4</v>
-      </c>
-      <c r="E100" s="4">
+      <c r="D100" s="2">
+        <v>4</v>
+      </c>
+      <c r="E100" s="2">
         <v>2</v>
       </c>
       <c r="F100" s="2"/>
@@ -3069,10 +3054,10 @@
       <c r="C101" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D101" s="4">
-        <v>4</v>
-      </c>
-      <c r="E101" s="4">
+      <c r="D101" s="2">
+        <v>4</v>
+      </c>
+      <c r="E101" s="2">
         <v>4</v>
       </c>
       <c r="F101" s="2"/>
@@ -3088,10 +3073,10 @@
       <c r="C102" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D102" s="2">
         <v>5</v>
       </c>
-      <c r="E102" s="4">
+      <c r="E102" s="2">
         <v>2</v>
       </c>
       <c r="F102" s="3" t="s">
@@ -3109,10 +3094,10 @@
       <c r="C103" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D103" s="4">
-        <v>3</v>
-      </c>
-      <c r="E103" s="4">
+      <c r="D103" s="2">
+        <v>3</v>
+      </c>
+      <c r="E103" s="2">
         <v>2</v>
       </c>
       <c r="F103" s="3" t="s">
@@ -3130,10 +3115,10 @@
       <c r="C104" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D104" s="4">
-        <v>2</v>
-      </c>
-      <c r="E104" s="4">
+      <c r="D104" s="2">
+        <v>2</v>
+      </c>
+      <c r="E104" s="2">
         <v>1</v>
       </c>
       <c r="F104" s="3" t="s">
@@ -3151,10 +3136,10 @@
       <c r="C105" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D105" s="4">
-        <v>3</v>
-      </c>
-      <c r="E105" s="4">
+      <c r="D105" s="2">
+        <v>3</v>
+      </c>
+      <c r="E105" s="2">
         <v>2</v>
       </c>
       <c r="F105" s="3" t="s">
@@ -3172,10 +3157,10 @@
       <c r="C106" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D106" s="2">
         <v>5</v>
       </c>
-      <c r="E106" s="4">
+      <c r="E106" s="2">
         <v>2</v>
       </c>
       <c r="F106" s="3" t="s">
@@ -3193,10 +3178,10 @@
       <c r="C107" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D107" s="4">
-        <v>4</v>
-      </c>
-      <c r="E107" s="4">
+      <c r="D107" s="2">
+        <v>4</v>
+      </c>
+      <c r="E107" s="2">
         <v>3</v>
       </c>
       <c r="F107" s="3" t="s">
@@ -3214,10 +3199,10 @@
       <c r="C108" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D108" s="4">
-        <v>2</v>
-      </c>
-      <c r="E108" s="4">
+      <c r="D108" s="2">
+        <v>2</v>
+      </c>
+      <c r="E108" s="2">
         <v>1</v>
       </c>
       <c r="F108" s="3" t="s">
@@ -3235,10 +3220,10 @@
       <c r="C109" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D109" s="4">
-        <v>8</v>
-      </c>
-      <c r="E109" s="4">
+      <c r="D109" s="2">
+        <v>8</v>
+      </c>
+      <c r="E109" s="2">
         <v>7</v>
       </c>
       <c r="F109" s="2"/>
@@ -3256,10 +3241,10 @@
       <c r="C110" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D110" s="4">
-        <v>4</v>
-      </c>
-      <c r="E110" s="4">
+      <c r="D110" s="2">
+        <v>4</v>
+      </c>
+      <c r="E110" s="2">
         <v>4</v>
       </c>
       <c r="F110" s="2"/>
@@ -3277,10 +3262,10 @@
       <c r="C111" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D111" s="4">
-        <v>3</v>
-      </c>
-      <c r="E111" s="4">
+      <c r="D111" s="2">
+        <v>3</v>
+      </c>
+      <c r="E111" s="2">
         <v>2</v>
       </c>
       <c r="F111" s="3" t="s">
@@ -3298,10 +3283,10 @@
       <c r="C112" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D112" s="2">
         <v>5</v>
       </c>
-      <c r="E112" s="4">
+      <c r="E112" s="2">
         <v>3</v>
       </c>
       <c r="F112" s="3" t="s">
@@ -3319,10 +3304,10 @@
       <c r="C113" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D113" s="4">
-        <v>4</v>
-      </c>
-      <c r="E113" s="4">
+      <c r="D113" s="2">
+        <v>4</v>
+      </c>
+      <c r="E113" s="2">
         <v>3</v>
       </c>
       <c r="F113" s="3" t="s">
@@ -3340,10 +3325,10 @@
       <c r="C114" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D114" s="4">
-        <v>4</v>
-      </c>
-      <c r="E114" s="4">
+      <c r="D114" s="2">
+        <v>4</v>
+      </c>
+      <c r="E114" s="2">
         <v>3</v>
       </c>
       <c r="F114" s="2"/>
@@ -3361,10 +3346,10 @@
       <c r="C115" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D115" s="4">
-        <v>2</v>
-      </c>
-      <c r="E115" s="4">
+      <c r="D115" s="2">
+        <v>2</v>
+      </c>
+      <c r="E115" s="2">
         <v>2</v>
       </c>
       <c r="F115" s="3" t="s">
@@ -3382,10 +3367,10 @@
       <c r="C116" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D116" s="2">
         <v>5</v>
       </c>
-      <c r="E116" s="4">
+      <c r="E116" s="2">
         <v>4</v>
       </c>
       <c r="F116" s="2"/>
@@ -3403,10 +3388,10 @@
       <c r="C117" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D117" s="2">
         <v>5</v>
       </c>
-      <c r="E117" s="4">
+      <c r="E117" s="2">
         <v>3</v>
       </c>
       <c r="F117" s="2"/>
@@ -3424,10 +3409,10 @@
       <c r="C118" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D118" s="2">
         <v>5</v>
       </c>
-      <c r="E118" s="4">
+      <c r="E118" s="2">
         <v>5</v>
       </c>
       <c r="F118" s="2"/>
@@ -3445,10 +3430,10 @@
       <c r="C119" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D119" s="2">
         <v>6</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119" s="2">
         <v>6</v>
       </c>
       <c r="F119" s="2"/>
@@ -3466,10 +3451,10 @@
       <c r="C120" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D120" s="4">
-        <v>3</v>
-      </c>
-      <c r="E120" s="4">
+      <c r="D120" s="2">
+        <v>3</v>
+      </c>
+      <c r="E120" s="2">
         <v>2</v>
       </c>
       <c r="F120" s="3" t="s">
@@ -3487,10 +3472,10 @@
       <c r="C121" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D121" s="4">
-        <v>4</v>
-      </c>
-      <c r="E121" s="4">
+      <c r="D121" s="2">
+        <v>4</v>
+      </c>
+      <c r="E121" s="2">
         <v>4</v>
       </c>
       <c r="F121" s="2"/>
@@ -3508,7 +3493,7 @@
       <c r="C122" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D122" s="2">
         <v>4</v>
       </c>
       <c r="E122" s="2"/>
@@ -3525,10 +3510,10 @@
       <c r="C123" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D123" s="4">
-        <v>3</v>
-      </c>
-      <c r="E123" s="4">
+      <c r="D123" s="2">
+        <v>3</v>
+      </c>
+      <c r="E123" s="2">
         <v>2</v>
       </c>
       <c r="F123" s="2"/>
@@ -3544,10 +3529,10 @@
       <c r="C124" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D124" s="4">
-        <v>3</v>
-      </c>
-      <c r="E124" s="4">
+      <c r="D124" s="2">
+        <v>3</v>
+      </c>
+      <c r="E124" s="2">
         <v>2</v>
       </c>
       <c r="F124" s="2"/>
@@ -3563,10 +3548,10 @@
       <c r="C125" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D125" s="2">
         <v>5</v>
       </c>
-      <c r="E125" s="4">
+      <c r="E125" s="2">
         <v>5</v>
       </c>
       <c r="F125" s="2"/>
@@ -3597,10 +3582,10 @@
       <c r="C127" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D127" s="2">
         <v>5</v>
       </c>
-      <c r="E127" s="4">
+      <c r="E127" s="2">
         <v>5</v>
       </c>
       <c r="F127" s="2"/>
@@ -3616,10 +3601,10 @@
       <c r="C128" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D128" s="2">
         <v>5</v>
       </c>
-      <c r="E128" s="4">
+      <c r="E128" s="2">
         <v>2</v>
       </c>
       <c r="F128" s="2"/>
@@ -3635,10 +3620,10 @@
       <c r="C129" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D129" s="4">
-        <v>3</v>
-      </c>
-      <c r="E129" s="4">
+      <c r="D129" s="2">
+        <v>3</v>
+      </c>
+      <c r="E129" s="2">
         <v>2</v>
       </c>
       <c r="F129" s="2"/>
@@ -3654,10 +3639,10 @@
       <c r="C130" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D130" s="4">
-        <v>3</v>
-      </c>
-      <c r="E130" s="4">
+      <c r="D130" s="2">
+        <v>3</v>
+      </c>
+      <c r="E130" s="2">
         <v>2</v>
       </c>
       <c r="F130" s="2"/>
@@ -3673,10 +3658,10 @@
       <c r="C131" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D131" s="4">
-        <v>3</v>
-      </c>
-      <c r="E131" s="4">
+      <c r="D131" s="2">
+        <v>3</v>
+      </c>
+      <c r="E131" s="2">
         <v>2</v>
       </c>
       <c r="F131" s="2"/>
@@ -3692,10 +3677,10 @@
       <c r="C132" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D132" s="4">
-        <v>3</v>
-      </c>
-      <c r="E132" s="4">
+      <c r="D132" s="2">
+        <v>3</v>
+      </c>
+      <c r="E132" s="2">
         <v>3</v>
       </c>
       <c r="F132" s="2"/>
@@ -3711,10 +3696,10 @@
       <c r="C133" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D133" s="2">
         <v>6</v>
       </c>
-      <c r="E133" s="4">
+      <c r="E133" s="2">
         <v>6</v>
       </c>
       <c r="F133" s="3" t="s">
@@ -3732,10 +3717,10 @@
       <c r="C134" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D134" s="2">
         <v>5</v>
       </c>
-      <c r="E134" s="4">
+      <c r="E134" s="2">
         <v>2</v>
       </c>
       <c r="F134" s="3" t="s">
@@ -3753,10 +3738,10 @@
       <c r="C135" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D135" s="4">
-        <v>2</v>
-      </c>
-      <c r="E135" s="4">
+      <c r="D135" s="2">
+        <v>2</v>
+      </c>
+      <c r="E135" s="2">
         <v>1</v>
       </c>
       <c r="F135" s="3" t="s">
@@ -3774,10 +3759,10 @@
       <c r="C136" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D136" s="4">
-        <v>3</v>
-      </c>
-      <c r="E136" s="4">
+      <c r="D136" s="2">
+        <v>3</v>
+      </c>
+      <c r="E136" s="2">
         <v>2</v>
       </c>
       <c r="F136" s="3" t="s">
@@ -3795,10 +3780,10 @@
       <c r="C137" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D137" s="4">
-        <v>3</v>
-      </c>
-      <c r="E137" s="4">
+      <c r="D137" s="2">
+        <v>3</v>
+      </c>
+      <c r="E137" s="2">
         <v>2</v>
       </c>
       <c r="F137" s="3" t="s">
@@ -3816,10 +3801,10 @@
       <c r="C138" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D138" s="4">
-        <v>2</v>
-      </c>
-      <c r="E138" s="4">
+      <c r="D138" s="2">
+        <v>2</v>
+      </c>
+      <c r="E138" s="2">
         <v>1</v>
       </c>
       <c r="F138" s="3" t="s">
@@ -3837,10 +3822,10 @@
       <c r="C139" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D139" s="4">
-        <v>2</v>
-      </c>
-      <c r="E139" s="4">
+      <c r="D139" s="2">
+        <v>2</v>
+      </c>
+      <c r="E139" s="2">
         <v>1</v>
       </c>
       <c r="F139" s="3" t="s">
@@ -3858,10 +3843,10 @@
       <c r="C140" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D140" s="2">
         <v>1</v>
       </c>
-      <c r="E140" s="4">
+      <c r="E140" s="2">
         <v>1</v>
       </c>
       <c r="F140" s="3" t="s">
@@ -3879,10 +3864,10 @@
       <c r="C141" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D141" s="4">
-        <v>3</v>
-      </c>
-      <c r="E141" s="4">
+      <c r="D141" s="2">
+        <v>3</v>
+      </c>
+      <c r="E141" s="2">
         <v>2</v>
       </c>
       <c r="F141" s="2"/>
@@ -3900,10 +3885,10 @@
       <c r="C142" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D142" s="2">
         <v>6</v>
       </c>
-      <c r="E142" s="4">
+      <c r="E142" s="2">
         <v>6</v>
       </c>
       <c r="F142" s="2"/>
@@ -3921,10 +3906,10 @@
       <c r="C143" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D143" s="4">
-        <v>4</v>
-      </c>
-      <c r="E143" s="4">
+      <c r="D143" s="2">
+        <v>4</v>
+      </c>
+      <c r="E143" s="2">
         <v>4</v>
       </c>
       <c r="F143" s="3" t="s">
@@ -3942,10 +3927,10 @@
       <c r="C144" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D144" s="4">
-        <v>3</v>
-      </c>
-      <c r="E144" s="4">
+      <c r="D144" s="2">
+        <v>3</v>
+      </c>
+      <c r="E144" s="2">
         <v>2</v>
       </c>
       <c r="F144" s="2"/>
@@ -3961,10 +3946,10 @@
       <c r="C145" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D145" s="4">
-        <v>4</v>
-      </c>
-      <c r="E145" s="4">
+      <c r="D145" s="2">
+        <v>4</v>
+      </c>
+      <c r="E145" s="2">
         <v>4</v>
       </c>
       <c r="F145" s="2"/>
@@ -3980,10 +3965,10 @@
       <c r="C146" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D146" s="4">
-        <v>2</v>
-      </c>
-      <c r="E146" s="4">
+      <c r="D146" s="2">
+        <v>2</v>
+      </c>
+      <c r="E146" s="2">
         <v>1</v>
       </c>
       <c r="F146" s="2"/>
@@ -3999,10 +3984,10 @@
       <c r="C147" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D147" s="2">
         <v>5</v>
       </c>
-      <c r="E147" s="4">
+      <c r="E147" s="2">
         <v>2</v>
       </c>
       <c r="F147" s="2"/>
@@ -4035,10 +4020,10 @@
       <c r="C149" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D149" s="4">
-        <v>4</v>
-      </c>
-      <c r="E149" s="4">
+      <c r="D149" s="2">
+        <v>4</v>
+      </c>
+      <c r="E149" s="2">
         <v>2</v>
       </c>
       <c r="F149" s="3" t="s">
@@ -4056,10 +4041,10 @@
       <c r="C150" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D150" s="4">
-        <v>4</v>
-      </c>
-      <c r="E150" s="4">
+      <c r="D150" s="2">
+        <v>4</v>
+      </c>
+      <c r="E150" s="2">
         <v>4</v>
       </c>
       <c r="F150" s="2"/>
@@ -4075,10 +4060,10 @@
       <c r="C151" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D151" s="4">
-        <v>2</v>
-      </c>
-      <c r="E151" s="4">
+      <c r="D151" s="2">
+        <v>2</v>
+      </c>
+      <c r="E151" s="2">
         <v>1</v>
       </c>
       <c r="F151" s="3" t="s">
@@ -4096,10 +4081,10 @@
       <c r="C152" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D152" s="2">
         <v>5</v>
       </c>
-      <c r="E152" s="4">
+      <c r="E152" s="2">
         <v>5</v>
       </c>
       <c r="F152" s="2"/>
@@ -4115,10 +4100,10 @@
       <c r="C153" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D153" s="4">
-        <v>3</v>
-      </c>
-      <c r="E153" s="4">
+      <c r="D153" s="2">
+        <v>3</v>
+      </c>
+      <c r="E153" s="2">
         <v>3</v>
       </c>
       <c r="F153" s="2"/>
@@ -4151,10 +4136,10 @@
       <c r="C155" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D155" s="2">
         <v>5</v>
       </c>
-      <c r="E155" s="4">
+      <c r="E155" s="2">
         <v>5</v>
       </c>
       <c r="F155" s="2"/>
@@ -4170,10 +4155,10 @@
       <c r="C156" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D156" s="4">
-        <v>4</v>
-      </c>
-      <c r="E156" s="4">
+      <c r="D156" s="2">
+        <v>4</v>
+      </c>
+      <c r="E156" s="2">
         <v>2</v>
       </c>
       <c r="F156" s="3" t="s">
@@ -4191,10 +4176,10 @@
       <c r="C157" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D157" s="4">
-        <v>2</v>
-      </c>
-      <c r="E157" s="4">
+      <c r="D157" s="2">
+        <v>2</v>
+      </c>
+      <c r="E157" s="2">
         <v>2</v>
       </c>
       <c r="F157" s="3" t="s">
@@ -4212,10 +4197,10 @@
       <c r="C158" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D158" s="4">
-        <v>3</v>
-      </c>
-      <c r="E158" s="4">
+      <c r="D158" s="2">
+        <v>3</v>
+      </c>
+      <c r="E158" s="2">
         <v>2</v>
       </c>
       <c r="F158" s="2"/>
@@ -4231,10 +4216,10 @@
       <c r="C159" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D159" s="2">
         <v>5</v>
       </c>
-      <c r="E159" s="4">
+      <c r="E159" s="2">
         <v>5</v>
       </c>
       <c r="F159" s="2"/>
@@ -4250,10 +4235,10 @@
       <c r="C160" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D160" s="4">
-        <v>2</v>
-      </c>
-      <c r="E160" s="4">
+      <c r="D160" s="2">
+        <v>2</v>
+      </c>
+      <c r="E160" s="2">
         <v>2</v>
       </c>
       <c r="F160" s="3" t="s">
@@ -4271,10 +4256,10 @@
       <c r="C161" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D161" s="4">
-        <v>3</v>
-      </c>
-      <c r="E161" s="4">
+      <c r="D161" s="2">
+        <v>3</v>
+      </c>
+      <c r="E161" s="2">
         <v>2</v>
       </c>
       <c r="F161" s="2"/>
@@ -4290,10 +4275,10 @@
       <c r="C162" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D162" s="4">
-        <v>4</v>
-      </c>
-      <c r="E162" s="4">
+      <c r="D162" s="2">
+        <v>4</v>
+      </c>
+      <c r="E162" s="2">
         <v>3</v>
       </c>
       <c r="F162" s="2"/>
@@ -4309,10 +4294,10 @@
       <c r="C163" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D163" s="4">
-        <v>4</v>
-      </c>
-      <c r="E163" s="4">
+      <c r="D163" s="2">
+        <v>4</v>
+      </c>
+      <c r="E163" s="2">
         <v>3</v>
       </c>
       <c r="F163" s="2"/>
@@ -4328,10 +4313,10 @@
       <c r="C164" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D164" s="4">
-        <v>3</v>
-      </c>
-      <c r="E164" s="4">
+      <c r="D164" s="2">
+        <v>3</v>
+      </c>
+      <c r="E164" s="2">
         <v>3</v>
       </c>
       <c r="F164" s="3" t="s">
@@ -4349,10 +4334,10 @@
       <c r="C165" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D165" s="4">
-        <v>2</v>
-      </c>
-      <c r="E165" s="4">
+      <c r="D165" s="2">
+        <v>2</v>
+      </c>
+      <c r="E165" s="2">
         <v>1</v>
       </c>
       <c r="F165" s="2"/>
@@ -4368,7 +4353,7 @@
       <c r="C166" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D166" s="2">
         <v>1</v>
       </c>
       <c r="E166" s="2"/>
@@ -4387,10 +4372,10 @@
       <c r="C167" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D167" s="2">
         <v>1</v>
       </c>
-      <c r="E167" s="4">
+      <c r="E167" s="2">
         <v>1</v>
       </c>
       <c r="F167" s="3" t="s">
@@ -4408,10 +4393,10 @@
       <c r="C168" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D168" s="2">
         <v>1</v>
       </c>
-      <c r="E168" s="4">
+      <c r="E168" s="2">
         <v>1</v>
       </c>
       <c r="F168" s="3" t="s">
@@ -4429,10 +4414,10 @@
       <c r="C169" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D169" s="4">
-        <v>2</v>
-      </c>
-      <c r="E169" s="4">
+      <c r="D169" s="2">
+        <v>2</v>
+      </c>
+      <c r="E169" s="2">
         <v>1</v>
       </c>
       <c r="F169" s="2"/>
@@ -4448,10 +4433,10 @@
       <c r="C170" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D170" s="2">
         <v>5</v>
       </c>
-      <c r="E170" s="4">
+      <c r="E170" s="2">
         <v>5</v>
       </c>
       <c r="F170" s="3" t="s">
@@ -4469,10 +4454,10 @@
       <c r="C171" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D171" s="4">
-        <v>3</v>
-      </c>
-      <c r="E171" s="4">
+      <c r="D171" s="2">
+        <v>3</v>
+      </c>
+      <c r="E171" s="2">
         <v>2</v>
       </c>
       <c r="F171" s="2"/>
@@ -4490,10 +4475,10 @@
       <c r="C172" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D172" s="4">
-        <v>4</v>
-      </c>
-      <c r="E172" s="4">
+      <c r="D172" s="2">
+        <v>4</v>
+      </c>
+      <c r="E172" s="2">
         <v>5</v>
       </c>
       <c r="F172" s="2"/>
@@ -4509,10 +4494,10 @@
       <c r="C173" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D173" s="4">
-        <v>2</v>
-      </c>
-      <c r="E173" s="4">
+      <c r="D173" s="2">
+        <v>2</v>
+      </c>
+      <c r="E173" s="2">
         <v>1</v>
       </c>
       <c r="F173" s="2"/>
@@ -4530,10 +4515,10 @@
       <c r="C174" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D174" s="2">
         <v>5</v>
       </c>
-      <c r="E174" s="4">
+      <c r="E174" s="2">
         <v>4</v>
       </c>
       <c r="F174" s="3" t="s">
@@ -4551,10 +4536,10 @@
       <c r="C175" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D175" s="4">
-        <v>2</v>
-      </c>
-      <c r="E175" s="4">
+      <c r="D175" s="2">
+        <v>2</v>
+      </c>
+      <c r="E175" s="2">
         <v>2</v>
       </c>
       <c r="F175" s="2"/>
@@ -4589,10 +4574,10 @@
       <c r="C177" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D177" s="2">
         <v>5</v>
       </c>
-      <c r="E177" s="4">
+      <c r="E177" s="2">
         <v>5</v>
       </c>
       <c r="F177" s="2"/>
@@ -4608,10 +4593,10 @@
       <c r="C178" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D178" s="4">
-        <v>2</v>
-      </c>
-      <c r="E178" s="4">
+      <c r="D178" s="2">
+        <v>2</v>
+      </c>
+      <c r="E178" s="2">
         <v>2</v>
       </c>
       <c r="F178" s="2"/>
@@ -4627,10 +4612,10 @@
       <c r="C179" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D179" s="2">
         <v>5</v>
       </c>
-      <c r="E179" s="4">
+      <c r="E179" s="2">
         <v>5</v>
       </c>
       <c r="F179" s="2"/>
@@ -4646,10 +4631,10 @@
       <c r="C180" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D180" s="4">
-        <v>2</v>
-      </c>
-      <c r="E180" s="4">
+      <c r="D180" s="2">
+        <v>2</v>
+      </c>
+      <c r="E180" s="2">
         <v>3</v>
       </c>
       <c r="F180" s="3" t="s">
@@ -4667,10 +4652,10 @@
       <c r="C181" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D181" s="4">
-        <v>2</v>
-      </c>
-      <c r="E181" s="4">
+      <c r="D181" s="2">
+        <v>2</v>
+      </c>
+      <c r="E181" s="2">
         <v>2</v>
       </c>
       <c r="F181" s="2"/>
@@ -4686,10 +4671,10 @@
       <c r="C182" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D182" s="2">
         <v>1</v>
       </c>
-      <c r="E182" s="4">
+      <c r="E182" s="2">
         <v>1</v>
       </c>
       <c r="F182" s="3" t="s">
@@ -4707,10 +4692,10 @@
       <c r="C183" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D183" s="4">
-        <v>3</v>
-      </c>
-      <c r="E183" s="4">
+      <c r="D183" s="2">
+        <v>3</v>
+      </c>
+      <c r="E183" s="2">
         <v>3</v>
       </c>
       <c r="F183" s="2"/>
@@ -4726,10 +4711,10 @@
       <c r="C184" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D184" s="4">
-        <v>4</v>
-      </c>
-      <c r="E184" s="4">
+      <c r="D184" s="2">
+        <v>4</v>
+      </c>
+      <c r="E184" s="2">
         <v>4</v>
       </c>
       <c r="F184" s="2"/>
@@ -4762,10 +4747,10 @@
       <c r="C186" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D186" s="4">
-        <v>4</v>
-      </c>
-      <c r="E186" s="4">
+      <c r="D186" s="2">
+        <v>4</v>
+      </c>
+      <c r="E186" s="2">
         <v>2</v>
       </c>
       <c r="F186" s="2"/>
@@ -4781,10 +4766,10 @@
       <c r="C187" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D187" s="4">
-        <v>4</v>
-      </c>
-      <c r="E187" s="4">
+      <c r="D187" s="2">
+        <v>4</v>
+      </c>
+      <c r="E187" s="2">
         <v>4</v>
       </c>
       <c r="F187" s="2"/>
@@ -4800,10 +4785,10 @@
       <c r="C188" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D188" s="4">
+      <c r="D188" s="2">
         <v>5</v>
       </c>
-      <c r="E188" s="4">
+      <c r="E188" s="2">
         <v>5</v>
       </c>
       <c r="F188" s="2"/>
@@ -4819,10 +4804,10 @@
       <c r="C189" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D189" s="4">
+      <c r="D189" s="2">
         <v>6</v>
       </c>
-      <c r="E189" s="4">
+      <c r="E189" s="2">
         <v>6</v>
       </c>
       <c r="F189" s="2"/>
@@ -4840,10 +4825,10 @@
       <c r="C190" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D190" s="4">
-        <v>2</v>
-      </c>
-      <c r="E190" s="4">
+      <c r="D190" s="2">
+        <v>2</v>
+      </c>
+      <c r="E190" s="2">
         <v>2</v>
       </c>
       <c r="F190" s="3" t="s">
@@ -4861,10 +4846,10 @@
       <c r="C191" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D191" s="4">
+      <c r="D191" s="2">
         <v>1</v>
       </c>
-      <c r="E191" s="4">
+      <c r="E191" s="2">
         <v>1</v>
       </c>
       <c r="F191" s="3" t="s">
@@ -4882,10 +4867,10 @@
       <c r="C192" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D192" s="4">
-        <v>2</v>
-      </c>
-      <c r="E192" s="4">
+      <c r="D192" s="2">
+        <v>2</v>
+      </c>
+      <c r="E192" s="2">
         <v>2</v>
       </c>
       <c r="F192" s="3" t="s">
@@ -4903,10 +4888,10 @@
       <c r="C193" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D193" s="4">
-        <v>3</v>
-      </c>
-      <c r="E193" s="4">
+      <c r="D193" s="2">
+        <v>3</v>
+      </c>
+      <c r="E193" s="2">
         <v>4</v>
       </c>
       <c r="F193" s="3" t="s">
@@ -4924,10 +4909,10 @@
       <c r="C194" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D194" s="4">
+      <c r="D194" s="2">
         <v>1</v>
       </c>
-      <c r="E194" s="4">
+      <c r="E194" s="2">
         <v>1</v>
       </c>
       <c r="F194" s="3" t="s">
@@ -4945,10 +4930,10 @@
       <c r="C195" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D195" s="4">
-        <v>2</v>
-      </c>
-      <c r="E195" s="4">
+      <c r="D195" s="2">
+        <v>2</v>
+      </c>
+      <c r="E195" s="2">
         <v>2</v>
       </c>
       <c r="F195" s="2"/>
@@ -4964,10 +4949,10 @@
       <c r="C196" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D196" s="4">
-        <v>4</v>
-      </c>
-      <c r="E196" s="4">
+      <c r="D196" s="2">
+        <v>4</v>
+      </c>
+      <c r="E196" s="2">
         <v>4</v>
       </c>
       <c r="F196" s="3" t="s">
@@ -4985,10 +4970,10 @@
       <c r="C197" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D197" s="4">
-        <v>2</v>
-      </c>
-      <c r="E197" s="4">
+      <c r="D197" s="2">
+        <v>2</v>
+      </c>
+      <c r="E197" s="2">
         <v>2</v>
       </c>
       <c r="F197" s="2"/>
@@ -5004,10 +4989,10 @@
       <c r="C198" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D198" s="4">
-        <v>2</v>
-      </c>
-      <c r="E198" s="4">
+      <c r="D198" s="2">
+        <v>2</v>
+      </c>
+      <c r="E198" s="2">
         <v>1</v>
       </c>
       <c r="F198" s="3" t="s">
@@ -5025,10 +5010,10 @@
       <c r="C199" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D199" s="4">
-        <v>4</v>
-      </c>
-      <c r="E199" s="4">
+      <c r="D199" s="2">
+        <v>4</v>
+      </c>
+      <c r="E199" s="2">
         <v>3</v>
       </c>
       <c r="F199" s="2"/>
@@ -5046,10 +5031,10 @@
       <c r="C200" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D200" s="4">
+      <c r="D200" s="2">
         <v>1</v>
       </c>
-      <c r="E200" s="4">
+      <c r="E200" s="2">
         <v>1</v>
       </c>
       <c r="F200" s="2"/>
@@ -5065,10 +5050,10 @@
       <c r="C201" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D201" s="4">
+      <c r="D201" s="2">
         <v>1</v>
       </c>
-      <c r="E201" s="4">
+      <c r="E201" s="2">
         <v>1</v>
       </c>
       <c r="F201" s="3" t="s">
@@ -5086,10 +5071,10 @@
       <c r="C202" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D202" s="4">
-        <v>8</v>
-      </c>
-      <c r="E202" s="4">
+      <c r="D202" s="2">
+        <v>8</v>
+      </c>
+      <c r="E202" s="2">
         <v>7</v>
       </c>
       <c r="F202" s="2"/>
@@ -5107,10 +5092,10 @@
       <c r="C203" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D203" s="4">
-        <v>2</v>
-      </c>
-      <c r="E203" s="4">
+      <c r="D203" s="2">
+        <v>2</v>
+      </c>
+      <c r="E203" s="2">
         <v>2</v>
       </c>
       <c r="F203" s="2"/>
@@ -5126,10 +5111,10 @@
       <c r="C204" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D204" s="4">
-        <v>2</v>
-      </c>
-      <c r="E204" s="4">
+      <c r="D204" s="2">
+        <v>2</v>
+      </c>
+      <c r="E204" s="2">
         <v>1</v>
       </c>
       <c r="F204" s="3" t="s">
@@ -5147,10 +5132,10 @@
       <c r="C205" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D205" s="4">
-        <v>4</v>
-      </c>
-      <c r="E205" s="4">
+      <c r="D205" s="2">
+        <v>4</v>
+      </c>
+      <c r="E205" s="2">
         <v>3</v>
       </c>
       <c r="F205" s="3" t="s">

</xml_diff>